<commit_message>
First commit with week 1,2,3
</commit_message>
<xml_diff>
--- a/Week_02/exercises/chicken_data.xlsx
+++ b/Week_02/exercises/chicken_data.xlsx
@@ -684,7 +684,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2435.836917152873</v>
+        <v>2606.416448354451</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2157.180544609028</v>
+        <v>3053.31058337847</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -712,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2558.418034509755</v>
+        <v>2847.640197843274</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -726,7 +726,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2679.200608096602</v>
+        <v>2459.147967212766</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -740,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2556.855145138803</v>
+        <v>2248.144178638431</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2749.335405965483</v>
+        <v>2257.849154695007</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -768,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2246.565466332238</v>
+        <v>2603.907684341763</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -782,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2959.190869729992</v>
+        <v>2025.798166228645</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -796,7 +796,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2728.468814160995</v>
+        <v>2390.981695750565</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -810,7 +810,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2449.062959399676</v>
+        <v>2727.393374112728</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -824,7 +824,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2196.644757527044</v>
+        <v>2413.774641403596</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -838,7 +838,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2504.121595305146</v>
+        <v>2089.423576260539</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -852,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2400.690361816204</v>
+        <v>2561.478901755176</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2635.299215849555</v>
+        <v>2627.327569072482</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -880,7 +880,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2512.049450608349</v>
+        <v>2730.563470972452</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -894,7 +894,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2548.551683322371</v>
+        <v>2696.586379383648</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -908,7 +908,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2613.606983816444</v>
+        <v>2550.983605975811</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -922,7 +922,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>2603.844751609005</v>
+        <v>2600.14071556693</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -936,7 +936,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>2258.823117658525</v>
+        <v>2420.024288839112</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -950,7 +950,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2586.092457619088</v>
+        <v>2154.203252790418</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -964,7 +964,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>2415.373741013068</v>
+        <v>2305.650715956946</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -978,7 +978,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>2315.352861083068</v>
+        <v>2881.905875171302</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -992,7 +992,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>2411.213526488157</v>
+        <v>3015.5767836972</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -1006,7 +1006,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>2707.369995982585</v>
+        <v>2606.543628668703</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1020,7 +1020,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>2828.033114144734</v>
+        <v>2447.78085163456</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -1034,7 +1034,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2805.739135758056</v>
+        <v>2528.232624638157</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -1048,7 +1048,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>2334.902532579886</v>
+        <v>2323.480365554033</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -1062,7 +1062,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>2700.569795953575</v>
+        <v>2403.23353332432</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1076,7 +1076,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>2216.46657649511</v>
+        <v>2706.704806540611</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>2674.342153167182</v>
+        <v>2471.872769223498</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -1104,7 +1104,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>2352.121480965922</v>
+        <v>2539.394945461609</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1118,7 +1118,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>2720.625199061993</v>
+        <v>3027.039581500004</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -1132,7 +1132,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>2927.473812362682</v>
+        <v>2776.507774859863</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>2219.88552286225</v>
+        <v>2494.761332372781</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -1160,7 +1160,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>2479.038035806728</v>
+        <v>2617.425363158868</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -1174,7 +1174,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>2095.447620693532</v>
+        <v>2408.512815481193</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1188,7 +1188,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>2316.371335305255</v>
+        <v>2722.326811720019</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -1202,7 +1202,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>2277.808500381769</v>
+        <v>2374.890503470433</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
@@ -1216,7 +1216,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>2708.372823419244</v>
+        <v>1703.402102931034</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1230,7 +1230,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>2419.522113597982</v>
+        <v>2580.988056903566</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1244,7 +1244,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>2559.902451574447</v>
+        <v>2450.994004403067</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -1258,7 +1258,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>2373.096997799733</v>
+        <v>3108.898085842262</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -1272,7 +1272,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>2813.339515670859</v>
+        <v>2470.12824808735</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -1286,7 +1286,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>2336.714468537502</v>
+        <v>2809.194562079102</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -1300,7 +1300,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>2499.189550963161</v>
+        <v>2720.817157426522</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -1314,7 +1314,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>3165.956792558491</v>
+        <v>2686.275312401783</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -1328,7 +1328,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>2375.659024484306</v>
+        <v>2436.191105308698</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -1342,7 +1342,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>2683.999631821952</v>
+        <v>2227.762205897822</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -1356,7 +1356,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>2270.759002694604</v>
+        <v>2132.204060600924</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -1370,7 +1370,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>2386.460316291711</v>
+        <v>2386.987192811604</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
@@ -1384,7 +1384,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>2411.413683034364</v>
+        <v>2234.665633016381</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
@@ -1398,7 +1398,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>1980.188220613222</v>
+        <v>2736.717304436537</v>
       </c>
       <c r="C53" t="s">
         <v>3</v>
@@ -1412,7 +1412,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>2061.673231776081</v>
+        <v>2503.349912097522</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
@@ -1426,7 +1426,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>2288.575436367175</v>
+        <v>2659.145710987831</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -1440,7 +1440,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>2400.344192119332</v>
+        <v>2833.446202761741</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -1454,7 +1454,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>2063.962021565017</v>
+        <v>2568.582053379174</v>
       </c>
       <c r="C57" t="s">
         <v>3</v>
@@ -1468,7 +1468,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>2351.912752193953</v>
+        <v>2605.053143552518</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -1482,7 +1482,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>2587.234531987627</v>
+        <v>2466.740220344659</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
@@ -1496,7 +1496,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>2597.946718573713</v>
+        <v>2453.699961771757</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -1510,7 +1510,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>2720.208329528295</v>
+        <v>2619.109955049199</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
@@ -1524,7 +1524,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>2264.112288476385</v>
+        <v>2087.589981833594</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -1538,7 +1538,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>2443.494437938852</v>
+        <v>2465.773663326734</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
@@ -1552,7 +1552,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>2549.443680121648</v>
+        <v>2420.125491387243</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
@@ -1566,7 +1566,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>2933.223660043263</v>
+        <v>2871.126459954377</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
@@ -1580,7 +1580,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>2544.096037928604</v>
+        <v>2488.411217610107</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
@@ -1594,7 +1594,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>2747.052614473884</v>
+        <v>2702.28057508017</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
@@ -1608,7 +1608,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>2756.049072383002</v>
+        <v>2834.165304847314</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
@@ -1622,7 +1622,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>1995.268720992748</v>
+        <v>2874.225766977246</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
@@ -1636,7 +1636,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>2721.741529605744</v>
+        <v>2329.805557297021</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -1650,7 +1650,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>3101.184169675052</v>
+        <v>2596.899551695898</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -1664,7 +1664,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>2237.994464245381</v>
+        <v>2535.842863725175</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -1678,7 +1678,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>2585.124156858858</v>
+        <v>2476.109109150387</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
@@ -1692,7 +1692,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>2401.339725534916</v>
+        <v>2635.381609629572</v>
       </c>
       <c r="C74" t="s">
         <v>0</v>
@@ -1706,7 +1706,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>2145.456781038363</v>
+        <v>2666.3581459758</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
@@ -1720,7 +1720,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>2512.675996338865</v>
+        <v>2464.991940481308</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
@@ -1734,7 +1734,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>2483.165499312508</v>
+        <v>2667.515458255037</v>
       </c>
       <c r="C77" t="s">
         <v>2</v>
@@ -1748,7 +1748,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>2480.321535060965</v>
+        <v>2261.297251888212</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
@@ -1762,7 +1762,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>2803.635402370798</v>
+        <v>2156.732763888876</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -1776,7 +1776,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>2479.062020985308</v>
+        <v>2380.855036120035</v>
       </c>
       <c r="C80" t="s">
         <v>4</v>
@@ -1790,7 +1790,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>2698.708061434907</v>
+        <v>2204.476163855022</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
@@ -1804,7 +1804,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>2253.844101819943</v>
+        <v>2419.577064306668</v>
       </c>
       <c r="C82" t="s">
         <v>4</v>
@@ -1818,7 +1818,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>2721.631003150052</v>
+        <v>2530.071181170762</v>
       </c>
       <c r="C83" t="s">
         <v>3</v>
@@ -1832,7 +1832,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>2674.675917214097</v>
+        <v>2676.690950262805</v>
       </c>
       <c r="C84" t="s">
         <v>2</v>
@@ -1846,7 +1846,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>2804.627274782364</v>
+        <v>2686.79899209044</v>
       </c>
       <c r="C85" t="s">
         <v>0</v>
@@ -1860,7 +1860,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>2062.533735395846</v>
+        <v>2515.713103419027</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
@@ -1874,7 +1874,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>2814.867887720169</v>
+        <v>2173.736883585239</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
@@ -1888,7 +1888,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>2414.638037314444</v>
+        <v>2463.656135190604</v>
       </c>
       <c r="C88" t="s">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>2283.506643128605</v>
+        <v>2417.50804182963</v>
       </c>
       <c r="C89" t="s">
         <v>3</v>
@@ -1916,7 +1916,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>2507.744559787777</v>
+        <v>2431.76083673618</v>
       </c>
       <c r="C90" t="s">
         <v>3</v>
@@ -1930,7 +1930,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>2235.94787703692</v>
+        <v>2126.855395295528</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -1944,7 +1944,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>2604.1220773692</v>
+        <v>2442.016240284512</v>
       </c>
       <c r="C92" t="s">
         <v>3</v>
@@ -1958,7 +1958,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>2483.91068518715</v>
+        <v>2073.189548946541</v>
       </c>
       <c r="C93" t="s">
         <v>0</v>
@@ -1972,7 +1972,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>2879.363471137186</v>
+        <v>2808.052179550587</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
@@ -1986,7 +1986,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>2509.057321974064</v>
+        <v>2599.775441453516</v>
       </c>
       <c r="C95" t="s">
         <v>2</v>
@@ -2000,7 +2000,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>2290.971897351606</v>
+        <v>2682.618647144555</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
@@ -2014,7 +2014,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>2657.234721949924</v>
+        <v>2247.319420936009</v>
       </c>
       <c r="C97" t="s">
         <v>2</v>
@@ -2028,7 +2028,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>2353.422440800807</v>
+        <v>2035.384321698455</v>
       </c>
       <c r="C98" t="s">
         <v>0</v>
@@ -2042,7 +2042,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>2681.538659293906</v>
+        <v>2779.233401436265</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
@@ -2056,7 +2056,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>2563.850789057699</v>
+        <v>2320.14829650485</v>
       </c>
       <c r="C100" t="s">
         <v>4</v>
@@ -2070,7 +2070,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>2342.702012511284</v>
+        <v>2259.48632838731</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>

</xml_diff>